<commit_message>
Excel parsing transform blank string to None
</commit_message>
<xml_diff>
--- a/features/fixtures/empty_cell_and_row.xlsx
+++ b/features/fixtures/empty_cell_and_row.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Next cell is none</t>
   </si>
@@ -23,10 +23,13 @@
     <t>Previous cell is none</t>
   </si>
   <si>
-    <t>Next cell is empty</t>
+    <t>The above row</t>
   </si>
   <si>
-    <t>Previous cell is empty</t>
+    <t>is full</t>
+  </si>
+  <si>
+    <t>of nones</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+      <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -149,8 +152,11 @@
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>3</v>
+      </c>
       <c r="C3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>